<commit_message>
remove 'Main Title' and switch subtitle to title, make cross-section naming simpler with only sheet and title
</commit_message>
<xml_diff>
--- a/templates/fields_template.xlsx
+++ b/templates/fields_template.xlsx
@@ -14,14 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>FIELDS Template</t>
   </si>
   <si>
-    <t>Subtitle</t>
-  </si>
-  <si>
     <t>Frequency (Hertz)</t>
   </si>
   <si>
@@ -100,13 +97,13 @@
     <t>Cross Section Tag</t>
   </si>
   <si>
-    <t>Main Title</t>
-  </si>
-  <si>
     <t>Ground Wire Tag</t>
   </si>
   <si>
     <t>Hot Wire Tag</t>
+  </si>
+  <si>
+    <t>Title</t>
   </si>
 </sst>
 </file>
@@ -184,13 +181,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -458,9 +455,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -482,21 +476,24 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -506,7 +503,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -616,7 +613,7 @@
     <c:title>
       <c:tx>
         <c:strRef>
-          <c:f>template!$B$5</c:f>
+          <c:f>template!$B$6</c:f>
           <c:strCache>
             <c:ptCount val="1"/>
           </c:strCache>
@@ -794,11 +791,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="112530560"/>
-        <c:axId val="112532480"/>
+        <c:axId val="68785280"/>
+        <c:axId val="68787200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="112530560"/>
+        <c:axId val="68785280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -823,12 +820,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112532480"/>
+        <c:crossAx val="68787200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="112532480"/>
+        <c:axId val="68787200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -854,7 +851,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112530560"/>
+        <c:crossAx val="68785280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -867,7 +864,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1196,7 +1193,7 @@
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1209,12 +1206,12 @@
     <col min="12" max="12" width="10.5703125" style="6" customWidth="1"/>
     <col min="13" max="14" width="10.5703125" style="9" customWidth="1"/>
     <col min="15" max="15" width="10.5703125" style="14" customWidth="1"/>
-    <col min="16" max="16" width="22.42578125" style="30" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.28515625" style="30" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="30"/>
+    <col min="16" max="16" width="22.42578125" style="29" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.28515625" style="29" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="28" customFormat="1" ht="15">
+    <row r="1" spans="1:17" s="27" customFormat="1" ht="15">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1231,9 +1228,9 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
-      <c r="O1" s="31"/>
-    </row>
-    <row r="2" spans="1:17" s="29" customFormat="1" ht="13.5" thickBot="1">
+      <c r="O1" s="30"/>
+    </row>
+    <row r="2" spans="1:17" s="28" customFormat="1" ht="13.5" thickBot="1">
       <c r="A2" s="3"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -1248,15 +1245,15 @@
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
-      <c r="O2" s="34"/>
+      <c r="O2" s="33"/>
     </row>
     <row r="3" spans="1:17" ht="15.75">
       <c r="A3" s="39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="40"/>
       <c r="C3" s="35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" s="36"/>
       <c r="E3" s="36"/>
@@ -1267,95 +1264,95 @@
       <c r="J3" s="36"/>
       <c r="K3" s="37"/>
       <c r="L3" s="35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M3" s="36"/>
       <c r="N3" s="36"/>
       <c r="O3" s="37"/>
       <c r="P3" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q3" s="38"/>
+    </row>
+    <row r="4" spans="1:17" ht="38.25">
+      <c r="A4" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="O4" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="P4" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="Q3" s="38"/>
-    </row>
-    <row r="4" spans="1:17" ht="38.25">
-      <c r="A4" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="L4" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="N4" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="O4" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="P4" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q4" s="26" t="s">
-        <v>17</v>
+      <c r="Q4" s="25" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" s="21" t="s">
-        <v>28</v>
+      <c r="A5" s="20" t="s">
+        <v>26</v>
       </c>
       <c r="B5" s="17"/>
       <c r="L5" s="9"/>
-      <c r="P5" s="27">
+      <c r="P5" s="26">
         <f>MAX(E5:E25,N5:N26)*1.05</f>
         <v>0</v>
       </c>
-      <c r="Q5" s="27">
-        <f>B13</f>
+      <c r="Q5" s="26">
+        <f>B12</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" s="21" t="s">
-        <v>27</v>
+      <c r="A6" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="B6" s="17"/>
       <c r="L6" s="9"/>
-      <c r="P6" s="27">
+      <c r="P6" s="26">
         <v>0</v>
       </c>
-      <c r="Q6" s="27">
-        <f>B13</f>
+      <c r="Q6" s="26">
+        <f>B12</f>
         <v>0</v>
       </c>
     </row>
@@ -1363,7 +1360,9 @@
       <c r="A7" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="17"/>
+      <c r="B7" s="34">
+        <v>60</v>
+      </c>
       <c r="C7" s="12"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
@@ -1374,9 +1373,9 @@
       <c r="J7" s="8"/>
       <c r="K7" s="15"/>
       <c r="L7" s="9"/>
-      <c r="P7" s="27"/>
-      <c r="Q7" s="27">
-        <f>B14</f>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="26">
+        <f>B13</f>
         <v>0</v>
       </c>
     </row>
@@ -1384,28 +1383,26 @@
       <c r="A8" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="18">
-        <v>60</v>
+      <c r="B8" s="34">
+        <v>100</v>
       </c>
       <c r="L8" s="9"/>
-      <c r="P8" s="27"/>
-      <c r="Q8" s="27">
-        <f>B14</f>
+      <c r="P8" s="26"/>
+      <c r="Q8" s="26">
+        <f>B13</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="18">
-        <v>100</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B9" s="17"/>
       <c r="L9" s="9"/>
     </row>
     <row r="10" spans="1:17">
       <c r="A10" s="16" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="12"/>
@@ -1421,25 +1418,25 @@
     </row>
     <row r="11" spans="1:17">
       <c r="A11" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="17"/>
+        <v>5</v>
+      </c>
+      <c r="B11" s="34">
+        <v>3</v>
+      </c>
       <c r="L11" s="9"/>
     </row>
     <row r="12" spans="1:17">
       <c r="A12" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="17"/>
+      <c r="L12" s="9"/>
+    </row>
+    <row r="13" spans="1:17" ht="13.5" thickBot="1">
+      <c r="A13" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="18">
-        <v>3</v>
-      </c>
-      <c r="L12" s="9"/>
-    </row>
-    <row r="13" spans="1:17">
-      <c r="A13" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="17"/>
+      <c r="B13" s="19"/>
       <c r="C13" s="12"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
@@ -1451,23 +1448,19 @@
       <c r="K13" s="15"/>
       <c r="L13" s="9"/>
     </row>
-    <row r="14" spans="1:17" ht="13.5" thickBot="1">
-      <c r="A14" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="20"/>
+    <row r="14" spans="1:17">
+      <c r="A14" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="42"/>
       <c r="L14" s="9"/>
     </row>
     <row r="15" spans="1:17" ht="12.75" customHeight="1">
-      <c r="A15" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="42"/>
+      <c r="A15" s="43"/>
+      <c r="B15" s="44"/>
       <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" s="43"/>
-      <c r="B16" s="44"/>
       <c r="C16" s="12"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
@@ -1535,15 +1528,15 @@
       <c r="N25"/>
     </row>
     <row r="26" spans="3:14">
-      <c r="C26" s="33"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="32"/>
-      <c r="K26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="31"/>
+      <c r="K26" s="31"/>
       <c r="L26" s="11"/>
       <c r="N26"/>
     </row>
@@ -1553,7 +1546,7 @@
     <mergeCell ref="L3:O3"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A15:B16"/>
+    <mergeCell ref="A14:B15"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>